<commit_message>
Update first page of excel sheet
</commit_message>
<xml_diff>
--- a/Assignment 3/shopping_platform.xlsx
+++ b/Assignment 3/shopping_platform.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarnebesjes/Documents/2023-2024/SE/practica/Software-Engineering-Practica/Assignment 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F7FC398-A5BF-594E-8639-E9203F1E3514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B99C1B1-69AC-2648-9FE8-670E1789FBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{C9565229-52D1-FB44-A940-46738BCA82DF}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{C9565229-52D1-FB44-A940-46738BCA82DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Critical Path Analysis" sheetId="2" r:id="rId1"/>
@@ -740,7 +740,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3D161E-32EE-0C41-B0E9-F1E5F055B4B0}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -775,7 +777,9 @@
       <c r="D2" s="18">
         <v>0</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -787,8 +791,12 @@
       <c r="C3" s="18">
         <v>2</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="D3" s="18">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -800,8 +808,12 @@
       <c r="C4" s="18">
         <v>3</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -813,8 +825,12 @@
       <c r="C5" s="18">
         <v>4</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="D5" s="18">
+        <v>3</v>
+      </c>
+      <c r="E5" s="18">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -826,8 +842,12 @@
       <c r="C6" s="18">
         <v>3</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="E6" s="18">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
@@ -839,8 +859,12 @@
       <c r="C7" s="18">
         <v>4</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="D7" s="18">
+        <v>7</v>
+      </c>
+      <c r="E7" s="18">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
@@ -852,8 +876,12 @@
       <c r="C8" s="18">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="18">
+        <v>6</v>
+      </c>
+      <c r="E8" s="18">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
@@ -865,8 +893,12 @@
       <c r="C9" s="18">
         <v>2</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="D9" s="18">
+        <v>6</v>
+      </c>
+      <c r="E9" s="18">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -878,8 +910,12 @@
       <c r="C10" s="18">
         <v>2</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="D10" s="18">
+        <v>10</v>
+      </c>
+      <c r="E10" s="18">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -891,8 +927,12 @@
       <c r="C11" s="18">
         <v>3</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="18">
+        <v>10</v>
+      </c>
+      <c r="E11" s="18">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -904,8 +944,12 @@
       <c r="C12" s="18">
         <v>2</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="18">
+        <v>13</v>
+      </c>
+      <c r="E12" s="18">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -916,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92443921-4E40-B148-875F-5DB41039A711}">
   <dimension ref="A1:T87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
@@ -2026,7 +2070,7 @@
         <v>18</v>
       </c>
       <c r="T20" s="16">
-        <f t="shared" ref="T3:T24" si="5">S20-R20</f>
+        <f t="shared" ref="T20:T21" si="5">S20-R20</f>
         <v>4</v>
       </c>
     </row>

</xml_diff>